<commit_message>
1, 3, 5, 10, 15, 20 year survival csv
</commit_message>
<xml_diff>
--- a/output/20_Year.xlsx
+++ b/output/20_Year.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kathleen/Courses/Berkeley-Data-Analytics/Class-Work/repos/transplant-survival/output/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{46FDC555-E623-6746-B234-4C071390A55B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A71D5F9C-B910-3F44-829D-D7C6D9E7E642}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="6780" yWindow="3800" windowWidth="26440" windowHeight="15440" xr2:uid="{634F7ABF-E449-9749-8622-A993FDFF144A}"/>
   </bookViews>
@@ -547,7 +547,7 @@
   <dimension ref="A1:AB122"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="J1" sqref="J1:K1048576"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>